<commit_message>
Added LCSC Part numbers for parts ordered
</commit_message>
<xml_diff>
--- a/Project Outputs for OpenScope_DigitalTest/BOM/OpenScope_DigitalTest_BOM.xlsx
+++ b/Project Outputs for OpenScope_DigitalTest/BOM/OpenScope_DigitalTest_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\OpenScope\OpenScope_DigitalTest\Project Outputs for OpenScope_DigitalTest\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD14B54-DE10-4707-B5C2-4F5B69FC6EF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90296E1-678F-4706-8093-0E267B8C2A3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FE443C88-A434-401A-8F0A-50795DCEAC8E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="241">
   <si>
     <t>Comment</t>
   </si>
@@ -612,9 +612,6 @@
     <t>Ultra Miniature Ceramic Glass Sealed SMD Cryastal, 12 MHz, 18 pF, +/- 20 ppm, -40 to 85 degC, 4-Pin SMD, RoHS, Tape and Reel</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
     <t>ABRACON_ABM8G_V</t>
   </si>
   <si>
@@ -688,13 +685,85 @@
   </si>
   <si>
     <t>C5, C6, C8, C9, C10, C11, C13, C14, C17, C19, C21, C27, C28, C29, C30, C31, C32, C33, C34, C35, C38, C41, C43, C44, C45, C46, C47, C48, C50, C52, C53, C54, C55, C58</t>
+  </si>
+  <si>
+    <t>CL10A105KA8NNNC</t>
+  </si>
+  <si>
+    <t>GRM188F51E104ZA01D</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R8BB104</t>
+  </si>
+  <si>
+    <t>GRM188R61A106ME69D</t>
+  </si>
+  <si>
+    <t>GRM155R61A106ME44D</t>
+  </si>
+  <si>
+    <t>CL05A475MQ5NRNC</t>
+  </si>
+  <si>
+    <t>0402CG180G500NT</t>
+  </si>
+  <si>
+    <t>LTST-C193KGKT-5A</t>
+  </si>
+  <si>
+    <t>LCSC Part Number</t>
+  </si>
+  <si>
+    <t>LTST-C193KRKT-5A</t>
+  </si>
+  <si>
+    <t>CR0603FA43R2G</t>
+  </si>
+  <si>
+    <t>WR06X101JTL</t>
+  </si>
+  <si>
+    <t>KH-SMA-K513-G</t>
+  </si>
+  <si>
+    <t>CBG160808U601T</t>
+  </si>
+  <si>
+    <t>WR06X4991FTL</t>
+  </si>
+  <si>
+    <t>0603WAF2201T5E</t>
+  </si>
+  <si>
+    <t>ARG03DTC1000</t>
+  </si>
+  <si>
+    <t>0603WAF1202T5E</t>
+  </si>
+  <si>
+    <t>MCT06030C1002FP500</t>
+  </si>
+  <si>
+    <t>TS5215A 160gf</t>
+  </si>
+  <si>
+    <t>C262918</t>
+  </si>
+  <si>
+    <t>C27882</t>
+  </si>
+  <si>
+    <t>C40955</t>
+  </si>
+  <si>
+    <t>C276421</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -710,8 +779,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,8 +801,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -776,11 +859,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDFDFDF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFDFDF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFDFDF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -801,8 +898,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1118,10 +1220,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,10 +1233,10 @@
     <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="13" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="14" max="14" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1174,8 +1276,11 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1209,8 +1314,11 @@
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1218,7 +1326,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -1244,8 +1352,11 @@
       </c>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1279,8 +1390,11 @@
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
@@ -1288,7 +1402,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>13</v>
@@ -1314,8 +1428,11 @@
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
@@ -1349,8 +1466,11 @@
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
@@ -1384,8 +1504,11 @@
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -1419,16 +1542,19 @@
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>57</v>
@@ -1454,8 +1580,11 @@
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>62</v>
       </c>
@@ -1475,7 +1604,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>60</v>
@@ -1489,8 +1618,11 @@
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>68</v>
       </c>
@@ -1522,8 +1654,11 @@
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>75</v>
       </c>
@@ -1557,8 +1692,11 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>82</v>
       </c>
@@ -1592,8 +1730,11 @@
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>89</v>
       </c>
@@ -1627,8 +1768,11 @@
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -1662,8 +1806,11 @@
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>103</v>
       </c>
@@ -1697,8 +1844,11 @@
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>108</v>
       </c>
@@ -1732,8 +1882,11 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N17" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>114</v>
       </c>
@@ -1767,8 +1920,11 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>119</v>
       </c>
@@ -1802,8 +1958,11 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>124</v>
       </c>
@@ -1837,8 +1996,11 @@
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>131</v>
       </c>
@@ -1876,8 +2038,11 @@
       <c r="M21" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>139</v>
       </c>
@@ -1916,7 +2081,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>147</v>
       </c>
@@ -1949,7 +2114,7 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>155</v>
       </c>
@@ -1984,7 +2149,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>161</v>
       </c>
@@ -2019,7 +2184,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>169</v>
       </c>
@@ -2057,8 +2222,11 @@
       <c r="M26" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>177</v>
       </c>
@@ -2093,7 +2261,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>183</v>
       </c>
@@ -2127,29 +2295,29 @@
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="F29" s="5">
         <v>1</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>190</v>
@@ -2158,96 +2326,124 @@
         <v>16</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>67</v>
       </c>
       <c r="M29" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>67</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>67</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL10A105KA8NNNC_1uF-105-10-25V_C5673.html" xr:uid="{82A381B4-0C98-4E30-B219-72ECFDC4483E}"/>
+    <hyperlink ref="N3" r:id="rId2" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_muRata_GRM188F51E104ZA01D_100nF-104-80-20-25V_C86002.html" xr:uid="{F9CC850E-07E6-4548-9274-80F8149AC32B}"/>
+    <hyperlink ref="N4" r:id="rId3" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_100nF-104-10-25V_C105883.html" xr:uid="{2458E02C-B8CB-4B9D-AD3E-94AD6CEA11A0}"/>
+    <hyperlink ref="N5" r:id="rId4" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_Murata-Electronics_GRM188R61A106ME69D_Murata-Electronics-GRM188R61A106ME69D_C90053.html" xr:uid="{0CCC9158-5DC2-4EC9-9F3C-170587A2CFE0}"/>
+    <hyperlink ref="N6" r:id="rId5" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_muRata_GRM155R61A106ME44D_10uF-106-20-10V_C77000.html" xr:uid="{647770C9-0027-40BA-8A74-28C2FF289978}"/>
+    <hyperlink ref="N7" r:id="rId6" display="https://lcsc.com/product-detail/Others_Samsung-Electro-Mechanics_CL05A475MQ5NRNC_Samsung-Electro-Mechanics-CL05A475MQ5NRNC_C307423.html" xr:uid="{4EC9D238-7316-458F-B36B-8B1E9884F033}"/>
+    <hyperlink ref="N8" r:id="rId7" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_FH-Guangdong-Fenghua-Advanced-Tech-0402CG180G500NT_C182481.html" xr:uid="{418E6D07-EA6B-4F36-B91C-4F1A40BF1A8B}"/>
+    <hyperlink ref="N9" r:id="rId8" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_SMD-green_C125102.html" xr:uid="{A66DBD8E-E01F-4D9F-BC52-61555EF600D4}"/>
+    <hyperlink ref="N10" r:id="rId9" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_SMD-red_C157741.html" xr:uid="{4FD5CEF0-C3BA-419D-A5BF-776CBD9B31F6}"/>
+    <hyperlink ref="N14" r:id="rId10" display="https://lcsc.com/product-detail/Resistors_LIZ-Elec-CR0603FA43R2G_C101046.html" xr:uid="{84C52300-01C2-4D80-B2FA-BA19E17763C5}"/>
+    <hyperlink ref="N19" r:id="rId11" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Walsin-Tech-Corp-WR06X101JTL_C163845.html" xr:uid="{91A530D8-35E5-49B6-BE31-A70FFF627F7A}"/>
+    <hyperlink ref="N11" r:id="rId12" display="https://lcsc.com/product-detail/RF-Connectors-Coaxial-Connectors_Shenzhen-Kinghelm-Elec-KH-SMA-K513-G_C411575.html" xr:uid="{20C32DFD-EFF8-48F8-A95B-ECED39DA9257}"/>
+    <hyperlink ref="N12" r:id="rId13" display="https://lcsc.com/product-detail/Ferrite-Beads_FH-Guangdong-Fenghua-Advanced-Tech-CBG160808U601T_C73326.html" xr:uid="{BB5C9335-63AD-43CB-95F3-E168024FDF8C}"/>
+    <hyperlink ref="N15" r:id="rId14" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Walsin-Tech-Corp-WR06X4991FTL_C163916.html" xr:uid="{72B8186E-D566-4E3D-9287-3BB39A74F494}"/>
+    <hyperlink ref="N16" r:id="rId15" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_UNI-ROYAL-Uniroyal-Elec-0603WAF2201T5E_C4190.html" xr:uid="{5790B7EE-24D0-48D8-AE06-4C18BE236A42}"/>
+    <hyperlink ref="N13" r:id="rId16" display="https://lcsc.com/product-detail/Others_Viking-Tech-ARG03DTC1000_C311907.html" xr:uid="{0F371208-0E35-41B3-8177-DFB64FC07CBD}"/>
+    <hyperlink ref="N17" r:id="rId17" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_UNI-ROYAL-Uniroyal-Elec-0603WAF1202T5E_C22790.html" xr:uid="{999443EF-DCC6-40E1-A2F0-1581F37F51F8}"/>
+    <hyperlink ref="N18" r:id="rId18" display="https://lcsc.com/product-detail/Others_Vishay-Intertech_MCT06030C1002FP500_Vishay-Intertech-MCT06030C1002FP500_C161803.html" xr:uid="{CBD53811-D5C1-4A5C-BB59-EE0D75C7E313}"/>
+    <hyperlink ref="N20" r:id="rId19" display="https://lcsc.com/product-detail/Tactile-Switches_SHOU-HAN-TS5215A-160gf_C412369.html" xr:uid="{1131122A-BAB8-4611-AB6A-8E908321F802}"/>
+    <hyperlink ref="N21" r:id="rId20" display="https://lcsc.com/product-detail/Others_STMicroelectronics_LD1086D2M33TR_STMicroelectronics-LD1086D2M33TR_C262918.html" xr:uid="{F8111A5D-8F28-4EFF-A1AD-E059A8BF85ED}"/>
+    <hyperlink ref="N26" r:id="rId21" display="https://lcsc.com/product-detail/USB-ICs_FTDI-Future-Designs_FT2232HL-REEL_FTDI-Future-Designs-FT2232HL-REEL_C27882.html" xr:uid="{818C1464-41E5-4E15-8F1C-9988EE617671}"/>
+    <hyperlink ref="N28" r:id="rId22" display="https://lcsc.com/product-detail/USB-Connectors_Jing-Extension-of-the-Electronic-Co-Jing-Extension-of-the-Electronic-Co-micro-5PBoard5-9No-column-plus-welding-feet-High-temperature_C40955.html" xr:uid="{C0EF39D7-3D1D-49D2-868E-6F68724829CA}"/>
+    <hyperlink ref="N29" r:id="rId23" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Abracon-LLC_ABM8G-12-000MHZ-B4Y-T_Abracon-LLC-ABM8G-12-000MHZ-B4Y-T_C276421.html" xr:uid="{769C7896-7115-4DFE-B721-F3F423BA3351}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="13" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="13" orientation="landscape" blackAndWhite="1" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>